<commit_message>
New data and transportation updates
</commit_message>
<xml_diff>
--- a/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
+++ b/InputData/elec/BTaDLP/BAU Trans and Distr Loss Perc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25525"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eltco\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE823980-A343-426D-B6F8-78088FFC2702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{DE823980-A343-426D-B6F8-78088FFC2702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86BC3202-C7F6-4B9F-A68F-7A125A829CDA}"/>
   <bookViews>
-    <workbookView xWindow="2556" yWindow="1104" windowWidth="15396" windowHeight="9972" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2556" yWindow="1104" windowWidth="15396" windowHeight="9972" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -59,43 +60,43 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>Canada's Energy Future</t>
+  </si>
+  <si>
+    <t>CER – Canada’s Energy Future 2020 (cer-rec.gc.ca)</t>
+  </si>
+  <si>
+    <t>CER – Canada’s Energy Future 2020 Supplement: Electricity (cer-rec.gc.ca)</t>
+  </si>
+  <si>
+    <t>Transmission losses</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Electricity generation, Canada, 2018 (GWh)</t>
+  </si>
+  <si>
+    <t>Canada Energy Futures 2020</t>
+  </si>
+  <si>
+    <t>Electricity end use, Canada, 2018 (PJ)</t>
+  </si>
+  <si>
+    <t>Electricity net export, Canada, 2018 (GWh)</t>
+  </si>
+  <si>
+    <t>Transmission losses (%)</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Transmission losses</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Electricity generation, Canada, 2018 (GWh)</t>
-  </si>
-  <si>
-    <t>Canada Energy Futures 2020</t>
-  </si>
-  <si>
-    <t>Electricity end use, Canada, 2018 (PJ)</t>
-  </si>
-  <si>
-    <t>Electricity net export, Canada, 2018 (GWh)</t>
-  </si>
-  <si>
-    <t>Transmission losses (%)</t>
-  </si>
-  <si>
-    <t>Calculated</t>
-  </si>
-  <si>
     <t>Trans and Dist Loss Perc (dimensionless)</t>
-  </si>
-  <si>
-    <t>Canada's Energy Future</t>
-  </si>
-  <si>
-    <t>CER – Canada’s Energy Future 2020 (cer-rec.gc.ca)</t>
-  </si>
-  <si>
-    <t>CER – Canada’s Energy Future 2020 Supplement: Electricity (cer-rec.gc.ca)</t>
   </si>
 </sst>
 </file>
@@ -104,9 +105,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,7 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -564,29 +565,29 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -603,103 +604,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39DFEA56-4608-4E0E-97F3-5D0584AC9F88}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B2" s="4">
         <v>643.51711</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4">
         <v>1999.61</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4">
         <v>46.815399999999997</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="7">
         <f>1-(B3+B4*3.6)/(B2*3.6)</f>
         <v>6.4107833555160365E-2</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4">
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="5"/>
@@ -718,19 +719,19 @@
   </sheetPr>
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>2018</v>
@@ -832,9 +833,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="28.9">
       <c r="A2" s="6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3">
         <f>Calculations!B5</f>
@@ -975,8 +976,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6681120aa8fa62dd7a0beb503524cb55">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b98e8ac0331400a99b3dbea3ee620024" ns2:_="" ns3:_="" ns4:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010010EB76B7FE121F489C7B2A4727FCE3E9" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fdee17017a9ad5b872047a216f95da93">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="52604411-7aeb-406e-8b34-4ce79a7293cc" xmlns:ns3="de340059-046a-4f1a-8b62-ade039df3700" xmlns:ns4="d580559a-617d-4d7d-8fb9-71ff64b58360" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37825e9edfcb807d863c63152c6d8635" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
     <xsd:import namespace="de340059-046a-4f1a-8b62-ade039df3700"/>
     <xsd:import namespace="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
@@ -1000,6 +1010,8 @@
                 <xsd:element ref="ns3:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns3:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1086,6 +1098,18 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceEventHashCode" ma:index="24" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="26" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="a296b89e-8abc-49db-b68e-edd9bb7809e5" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="27" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -1220,15 +1244,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1242,36 +1257,21 @@
       <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     </l787e5950a9249679d0130235a9a791b>
     <TaxCatchAll xmlns="52604411-7aeb-406e-8b34-4ce79a7293cc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de340059-046a-4f1a-8b62-ade039df3700">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3EFCE222-B7D0-45BD-A68C-86B8A9E04625}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE709384-6DCD-4D87-933A-B602BAF01A51}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE709384-6DCD-4D87-933A-B602BAF01A51}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DEBBA6BA-06D7-4E0F-9F0A-CC9345FF7E89}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B92A9A08-A155-488A-AEC9-C41D794AC0DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="de340059-046a-4f1a-8b62-ade039df3700"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d580559a-617d-4d7d-8fb9-71ff64b58360"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="52604411-7aeb-406e-8b34-4ce79a7293cc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B92A9A08-A155-488A-AEC9-C41D794AC0DD}"/>
 </file>
</xml_diff>